<commit_message>
Mise à jour des formats in (had, mco, rafael, ssr, psy) hors les anohosp (formats non encore disponibles le 27 février 2022).
</commit_message>
<xml_diff>
--- a/formats/excel/MCO/2022/Formats RUM 22.xlsx
+++ b/formats/excel/MCO/2022/Formats RUM 22.xlsx
@@ -444,20 +444,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C38" activeCellId="0" sqref="C38"/>
+      <selection pane="topLeft" activeCell="F39" activeCellId="0" sqref="F39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.9921875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="46.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="10.5"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -477,7 +478,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
@@ -498,7 +499,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>3</v>
       </c>
@@ -519,7 +520,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>9</v>
       </c>
@@ -537,7 +538,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>10</v>
       </c>
@@ -558,7 +559,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>13</v>
       </c>
@@ -579,7 +580,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>16</v>
       </c>
@@ -600,7 +601,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>25</v>
       </c>
@@ -621,7 +622,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>28</v>
       </c>
@@ -642,7 +643,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>48</v>
       </c>
@@ -663,7 +664,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>68</v>
       </c>
@@ -684,7 +685,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>78</v>
       </c>
@@ -705,7 +706,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>86</v>
       </c>
@@ -726,7 +727,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>87</v>
       </c>
@@ -747,7 +748,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>91</v>
       </c>
@@ -768,7 +769,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>93</v>
       </c>
@@ -789,7 +790,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>101</v>
       </c>
@@ -810,7 +811,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>102</v>
       </c>
@@ -831,7 +832,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>103</v>
       </c>
@@ -852,7 +853,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
         <v>111</v>
       </c>
@@ -873,7 +874,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <v>112</v>
       </c>
@@ -894,7 +895,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
         <v>113</v>
       </c>
@@ -915,7 +916,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
         <v>118</v>
       </c>
@@ -936,7 +937,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
         <v>122</v>
       </c>
@@ -957,7 +958,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
         <v>124</v>
       </c>
@@ -978,7 +979,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
         <v>132</v>
       </c>
@@ -999,7 +1000,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
         <v>134</v>
       </c>
@@ -1020,7 +1021,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
         <v>136</v>
       </c>
@@ -1041,7 +1042,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
         <v>138</v>
       </c>
@@ -1062,7 +1063,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
         <v>141</v>
       </c>
@@ -1083,7 +1084,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
         <v>149</v>
       </c>
@@ -1104,7 +1105,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
         <v>157</v>
       </c>
@@ -1125,7 +1126,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
         <v>160</v>
       </c>
@@ -1146,7 +1147,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
         <v>161</v>
       </c>
@@ -1167,7 +1168,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
         <v>162</v>
       </c>
@@ -1188,7 +1189,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
         <v>163</v>
       </c>
@@ -1209,7 +1210,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
         <v>178</v>
       </c>
@@ -1230,7 +1231,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
         <v>179</v>
       </c>
@@ -1251,7 +1252,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
         <v>180</v>
       </c>
@@ -1271,9 +1272,8 @@
       <c r="F39" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="G39" s="3"/>
-    </row>
-    <row r="40" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
         <v>181</v>
       </c>
@@ -1293,7 +1293,6 @@
       <c r="F40" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="G40" s="3"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
@@ -1315,7 +1314,6 @@
       <c r="F41" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="G41" s="3"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
@@ -1337,7 +1335,6 @@
       <c r="F42" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="G42" s="3"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
@@ -1359,7 +1356,6 @@
       <c r="F43" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="G43" s="4"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
@@ -1379,7 +1375,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="n">
         <v>190</v>
       </c>
@@ -1400,7 +1396,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="n">
         <v>193</v>
       </c>
@@ -1415,13 +1411,6 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="F43:G43"/>
-  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>